<commit_message>
Humidity spline parametrization attempts
ParametrizeHumidity class updated with new geometry options.
Added pressure to saturation vapor calculation.
</commit_message>
<xml_diff>
--- a/data/weather/standard_profiles/Standard Profiles.xlsx
+++ b/data/weather/standard_profiles/Standard Profiles.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\GitHub\weather\data\weather\twister\standard_profiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\GitHub\weather\data\weather\standard_profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6068BCC-367C-4182-8990-E9D6F2457BBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C233A0-E4A2-4A57-ACCD-EBC3BD5F41C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="11550" xr2:uid="{E751E42B-8441-4F50-9123-C41EFFF043F1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25598" windowHeight="11550" activeTab="2" xr2:uid="{E751E42B-8441-4F50-9123-C41EFFF043F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Standard Temperature" sheetId="1" r:id="rId1"/>
     <sheet name="Standard Relative Humidity" sheetId="2" r:id="rId2"/>
+    <sheet name="Standard Pressure" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>Temperature</t>
   </si>
@@ -41,12 +42,28 @@
   <si>
     <t>Relative Humidity</t>
   </si>
+  <si>
+    <t>Pressure</t>
+  </si>
+  <si>
+    <t>(Pa)</t>
+  </si>
+  <si>
+    <t>(10^4 Pa)</t>
+  </si>
+  <si>
+    <t>(hPa)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,13 +90,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -106,11 +135,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -136,8 +166,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -453,16 +509,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA2C154-3D99-44ED-96DE-9D924935FB2F}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
@@ -474,7 +530,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="9">
         <v>-1000</v>
       </c>
@@ -486,7 +542,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="10">
         <v>0</v>
       </c>
@@ -498,7 +554,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="10">
         <v>1000</v>
       </c>
@@ -510,7 +566,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="10">
         <v>2000</v>
       </c>
@@ -522,7 +578,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="10">
         <v>3000</v>
       </c>
@@ -534,7 +590,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="10">
         <v>4000</v>
       </c>
@@ -546,7 +602,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="10">
         <v>5000</v>
       </c>
@@ -558,7 +614,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="10">
         <v>6000</v>
       </c>
@@ -570,7 +626,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="10">
         <v>7000</v>
       </c>
@@ -582,7 +638,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="10">
         <v>8000</v>
       </c>
@@ -594,7 +650,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="10">
         <v>9000</v>
       </c>
@@ -606,7 +662,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="10">
         <v>10000</v>
       </c>
@@ -618,7 +674,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="10">
         <v>15000</v>
       </c>
@@ -630,7 +686,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="10">
         <v>20000</v>
       </c>
@@ -642,7 +698,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="10">
         <v>25000</v>
       </c>
@@ -654,7 +710,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="10">
         <v>30000</v>
       </c>
@@ -666,7 +722,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="10">
         <v>40000</v>
       </c>
@@ -678,7 +734,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="10">
         <v>50000</v>
       </c>
@@ -690,7 +746,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="10">
         <v>60000</v>
       </c>
@@ -702,7 +758,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="10">
         <v>70000</v>
       </c>
@@ -714,7 +770,7 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="10">
         <v>80000</v>
       </c>
@@ -726,7 +782,7 @@
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="7"/>
@@ -748,12 +804,12 @@
       <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -761,7 +817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -769,7 +825,7 @@
         <v>59.62</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="3">
         <v>304.8</v>
       </c>
@@ -777,7 +833,7 @@
         <v>60.48</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
         <v>609.6</v>
       </c>
@@ -785,7 +841,7 @@
         <v>62.03</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="3">
         <v>914.4</v>
       </c>
@@ -793,7 +849,7 @@
         <v>63.83</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="3">
         <v>1219.2</v>
       </c>
@@ -801,7 +857,7 @@
         <v>65.569999999999993</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="3">
         <v>1524</v>
       </c>
@@ -809,7 +865,7 @@
         <v>67.06</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="3">
         <v>1828.8</v>
       </c>
@@ -817,7 +873,7 @@
         <v>68.2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="3">
         <v>2133.6</v>
       </c>
@@ -825,7 +881,7 @@
         <v>68.97</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="3">
         <v>2438.4</v>
       </c>
@@ -833,7 +889,7 @@
         <v>69.41</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="3">
         <v>2743.2</v>
       </c>
@@ -841,7 +897,7 @@
         <v>69.62</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="3">
         <v>3048</v>
       </c>
@@ -849,7 +905,7 @@
         <v>69.72</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="3">
         <v>3352.8</v>
       </c>
@@ -857,7 +913,7 @@
         <v>69.83</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="3">
         <v>3657.6</v>
       </c>
@@ -865,7 +921,7 @@
         <v>70.05</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="3">
         <v>3962.4</v>
       </c>
@@ -873,7 +929,7 @@
         <v>70.459999999999994</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="3">
         <v>4267.2</v>
       </c>
@@ -881,7 +937,7 @@
         <v>71.12</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="3">
         <v>4572</v>
       </c>
@@ -889,7 +945,7 @@
         <v>72.040000000000006</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="3">
         <v>4876.8</v>
       </c>
@@ -897,7 +953,7 @@
         <v>73.19</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="3">
         <v>5181.6000000000004</v>
       </c>
@@ -905,7 +961,7 @@
         <v>74.48</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="3">
         <v>5486.4</v>
       </c>
@@ -913,7 +969,7 @@
         <v>75.77</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="3">
         <v>5791.2</v>
       </c>
@@ -921,7 +977,7 @@
         <v>76.900000000000006</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" s="3">
         <v>6096</v>
       </c>
@@ -929,7 +985,7 @@
         <v>77.61</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="3">
         <v>6400.8</v>
       </c>
@@ -937,7 +993,7 @@
         <v>77.66</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" s="3">
         <v>6705.6</v>
       </c>
@@ -945,7 +1001,7 @@
         <v>76.77</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" s="3">
         <v>7010.4</v>
       </c>
@@ -953,7 +1009,7 @@
         <v>74.75</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" s="3">
         <v>7315.2</v>
       </c>
@@ -961,7 +1017,7 @@
         <v>71.47</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="3">
         <v>7620</v>
       </c>
@@ -969,7 +1025,7 @@
         <v>66.959999999999994</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" s="3">
         <v>7924.8</v>
       </c>
@@ -977,7 +1033,7 @@
         <v>61.38</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" s="3">
         <v>8229.6</v>
       </c>
@@ -985,7 +1041,7 @@
         <v>55.07</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" s="3">
         <v>8534.4</v>
       </c>
@@ -993,7 +1049,7 @@
         <v>48.44</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" s="3">
         <v>8839.2000000000007</v>
       </c>
@@ -1001,7 +1057,7 @@
         <v>41.95</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" s="3">
         <v>9144</v>
       </c>
@@ -1009,7 +1065,7 @@
         <v>36.01</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" s="3">
         <v>9448.7999999999993</v>
       </c>
@@ -1017,7 +1073,7 @@
         <v>30.95</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="3">
         <v>9753.6</v>
       </c>
@@ -1025,7 +1081,7 @@
         <v>27.01</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" s="3">
         <v>10058.4</v>
       </c>
@@ -1033,7 +1089,7 @@
         <v>24.38</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="3">
         <v>10363.200000000001</v>
       </c>
@@ -1041,7 +1097,7 @@
         <v>23.31</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" s="3">
         <v>10668</v>
       </c>
@@ -1049,7 +1105,7 @@
         <v>24.29</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" s="3">
         <v>10972.8</v>
       </c>
@@ -1057,7 +1113,7 @@
         <v>28.6</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" s="3">
         <v>11277.6</v>
       </c>
@@ -1065,7 +1121,7 @@
         <v>25.61</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" s="3">
         <v>11582.4</v>
       </c>
@@ -1073,7 +1129,7 @@
         <v>22.1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="3">
         <v>11887.2</v>
       </c>
@@ -1081,7 +1137,7 @@
         <v>19.04</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" s="3">
         <v>12192</v>
       </c>
@@ -1089,7 +1145,7 @@
         <v>16.420000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" s="3">
         <v>12496.8</v>
       </c>
@@ -1097,7 +1153,7 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44" s="3">
         <v>12801.6</v>
       </c>
@@ -1105,7 +1161,7 @@
         <v>12.34</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" s="3">
         <v>13106.4</v>
       </c>
@@ -1113,7 +1169,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A46" s="3">
         <v>13411.2</v>
       </c>
@@ -1121,7 +1177,7 @@
         <v>9.5299999999999994</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47" s="3">
         <v>13716</v>
       </c>
@@ -1129,7 +1185,7 @@
         <v>8.49</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48" s="3">
         <v>14020.8</v>
       </c>
@@ -1137,7 +1193,7 @@
         <v>7.64</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A49" s="3">
         <v>14325.6</v>
       </c>
@@ -1145,7 +1201,7 @@
         <v>6.95</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A50" s="3">
         <v>14630.4</v>
       </c>
@@ -1153,7 +1209,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A51" s="3">
         <v>14935.2</v>
       </c>
@@ -1161,7 +1217,7 @@
         <v>5.97</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A52" s="3">
         <v>15240</v>
       </c>
@@ -1169,7 +1225,7 @@
         <v>5.63</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A53" s="3">
         <v>15544.8</v>
       </c>
@@ -1177,7 +1233,7 @@
         <v>5.38</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A54" s="3">
         <v>16154.4</v>
       </c>
@@ -1185,7 +1241,7 @@
         <v>5.08</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A55" s="3">
         <v>16459.2</v>
       </c>
@@ -1193,7 +1249,7 @@
         <v>5.0199999999999996</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A56" s="3">
         <v>16764</v>
       </c>
@@ -1201,7 +1257,7 @@
         <v>5.01</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A57" s="3">
         <v>17068.8</v>
       </c>
@@ -1209,7 +1265,7 @@
         <v>5.03</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A58" s="3">
         <v>17373.599999999999</v>
       </c>
@@ -1217,7 +1273,7 @@
         <v>5.09</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A59" s="3">
         <v>17678.400000000001</v>
       </c>
@@ -1225,7 +1281,7 @@
         <v>5.18</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A60" s="3">
         <v>17983.2</v>
       </c>
@@ -1233,7 +1289,7 @@
         <v>5.28</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A61" s="3">
         <v>18288</v>
       </c>
@@ -1241,7 +1297,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A62" s="3">
         <v>18592.8</v>
       </c>
@@ -1252,4 +1308,549 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{139701CB-2514-4CE1-B94F-F59E40FB8BD3}">
+  <dimension ref="A1:L24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.9296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A2" s="18">
+        <v>-1000</v>
+      </c>
+      <c r="B2" s="17">
+        <f>C2/100</f>
+        <v>1139</v>
+      </c>
+      <c r="C2" s="16">
+        <f>10000*D2</f>
+        <v>113900</v>
+      </c>
+      <c r="D2" s="10">
+        <v>11.39</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A3" s="19">
+        <v>0</v>
+      </c>
+      <c r="B3" s="17">
+        <f t="shared" ref="B3:B22" si="0">C3/100</f>
+        <v>1013.0000000000001</v>
+      </c>
+      <c r="C3" s="16">
+        <f t="shared" ref="C3:C22" si="1">10000*D3</f>
+        <v>101300.00000000001</v>
+      </c>
+      <c r="D3" s="12">
+        <v>10.130000000000001</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A4" s="19">
+        <v>1000</v>
+      </c>
+      <c r="B4" s="17">
+        <f t="shared" si="0"/>
+        <v>898.8</v>
+      </c>
+      <c r="C4" s="16">
+        <f t="shared" si="1"/>
+        <v>89880</v>
+      </c>
+      <c r="D4" s="12">
+        <v>8.9879999999999995</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A5" s="19">
+        <v>2000</v>
+      </c>
+      <c r="B5" s="17">
+        <f t="shared" si="0"/>
+        <v>795</v>
+      </c>
+      <c r="C5" s="16">
+        <f t="shared" si="1"/>
+        <v>79500</v>
+      </c>
+      <c r="D5" s="12">
+        <v>7.95</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A6" s="19">
+        <v>3000</v>
+      </c>
+      <c r="B6" s="17">
+        <f t="shared" si="0"/>
+        <v>701.2</v>
+      </c>
+      <c r="C6" s="16">
+        <f t="shared" si="1"/>
+        <v>70120</v>
+      </c>
+      <c r="D6" s="12">
+        <v>7.0119999999999996</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A7" s="19">
+        <v>4000</v>
+      </c>
+      <c r="B7" s="17">
+        <f t="shared" si="0"/>
+        <v>616.6</v>
+      </c>
+      <c r="C7" s="16">
+        <f t="shared" si="1"/>
+        <v>61660.000000000007</v>
+      </c>
+      <c r="D7" s="12">
+        <v>6.1660000000000004</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A8" s="19">
+        <v>5000</v>
+      </c>
+      <c r="B8" s="17">
+        <f t="shared" si="0"/>
+        <v>540.5</v>
+      </c>
+      <c r="C8" s="16">
+        <f t="shared" si="1"/>
+        <v>54050</v>
+      </c>
+      <c r="D8" s="12">
+        <v>5.4050000000000002</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A9" s="19">
+        <v>6000</v>
+      </c>
+      <c r="B9" s="17">
+        <f t="shared" si="0"/>
+        <v>472.20000000000005</v>
+      </c>
+      <c r="C9" s="16">
+        <f t="shared" si="1"/>
+        <v>47220.000000000007</v>
+      </c>
+      <c r="D9" s="12">
+        <v>4.7220000000000004</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A10" s="19">
+        <v>7000</v>
+      </c>
+      <c r="B10" s="17">
+        <f t="shared" si="0"/>
+        <v>411.1</v>
+      </c>
+      <c r="C10" s="16">
+        <f t="shared" si="1"/>
+        <v>41110</v>
+      </c>
+      <c r="D10" s="12">
+        <v>4.1109999999999998</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A11" s="19">
+        <v>8000</v>
+      </c>
+      <c r="B11" s="17">
+        <f t="shared" si="0"/>
+        <v>356.5</v>
+      </c>
+      <c r="C11" s="16">
+        <f t="shared" si="1"/>
+        <v>35650</v>
+      </c>
+      <c r="D11" s="12">
+        <v>3.5649999999999999</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A12" s="19">
+        <v>9000</v>
+      </c>
+      <c r="B12" s="17">
+        <f t="shared" si="0"/>
+        <v>308</v>
+      </c>
+      <c r="C12" s="16">
+        <f t="shared" si="1"/>
+        <v>30800</v>
+      </c>
+      <c r="D12" s="12">
+        <v>3.08</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A13" s="19">
+        <v>10000</v>
+      </c>
+      <c r="B13" s="17">
+        <f t="shared" si="0"/>
+        <v>265</v>
+      </c>
+      <c r="C13" s="16">
+        <f t="shared" si="1"/>
+        <v>26500</v>
+      </c>
+      <c r="D13" s="12">
+        <v>2.65</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A14" s="19">
+        <v>15000</v>
+      </c>
+      <c r="B14" s="17">
+        <f t="shared" si="0"/>
+        <v>121.1</v>
+      </c>
+      <c r="C14" s="16">
+        <f t="shared" si="1"/>
+        <v>12110</v>
+      </c>
+      <c r="D14" s="12">
+        <v>1.2110000000000001</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A15" s="19">
+        <v>20000</v>
+      </c>
+      <c r="B15" s="17">
+        <f t="shared" si="0"/>
+        <v>55.289999999999992</v>
+      </c>
+      <c r="C15" s="16">
+        <f t="shared" si="1"/>
+        <v>5528.9999999999991</v>
+      </c>
+      <c r="D15" s="12">
+        <v>0.55289999999999995</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A16" s="19">
+        <v>25000</v>
+      </c>
+      <c r="B16" s="17">
+        <f t="shared" si="0"/>
+        <v>25.49</v>
+      </c>
+      <c r="C16" s="16">
+        <f t="shared" si="1"/>
+        <v>2549</v>
+      </c>
+      <c r="D16" s="12">
+        <v>0.25490000000000002</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A17" s="19">
+        <v>30000</v>
+      </c>
+      <c r="B17" s="17">
+        <f t="shared" si="0"/>
+        <v>11.97</v>
+      </c>
+      <c r="C17" s="16">
+        <f t="shared" si="1"/>
+        <v>1197</v>
+      </c>
+      <c r="D17" s="12">
+        <v>0.1197</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A18" s="19">
+        <v>40000</v>
+      </c>
+      <c r="B18" s="17">
+        <f t="shared" si="0"/>
+        <v>2.87</v>
+      </c>
+      <c r="C18" s="16">
+        <f t="shared" si="1"/>
+        <v>287</v>
+      </c>
+      <c r="D18" s="13">
+        <v>2.87E-2</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A19" s="19">
+        <v>50000</v>
+      </c>
+      <c r="B19" s="17">
+        <f t="shared" si="0"/>
+        <v>0.79780000000000006</v>
+      </c>
+      <c r="C19" s="16">
+        <f t="shared" si="1"/>
+        <v>79.78</v>
+      </c>
+      <c r="D19" s="12">
+        <v>7.9780000000000007E-3</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A20" s="19">
+        <v>60000</v>
+      </c>
+      <c r="B20" s="17">
+        <f t="shared" si="0"/>
+        <v>0.21960000000000002</v>
+      </c>
+      <c r="C20" s="16">
+        <f t="shared" si="1"/>
+        <v>21.96</v>
+      </c>
+      <c r="D20" s="12">
+        <v>2.196E-3</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A21" s="19">
+        <v>70000</v>
+      </c>
+      <c r="B21" s="17">
+        <f t="shared" si="0"/>
+        <v>5.1999999999999991E-2</v>
+      </c>
+      <c r="C21" s="16">
+        <f t="shared" si="1"/>
+        <v>5.1999999999999993</v>
+      </c>
+      <c r="D21" s="12">
+        <v>5.1999999999999995E-4</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A22" s="19">
+        <v>80000</v>
+      </c>
+      <c r="B22" s="17">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="C22" s="16">
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D22" s="12">
+        <v>1.1E-4</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to ParametrizeHumidity class and Autoencoder Added
Geometry updates for ParametrizeHumidity class along with bug fixes.
Autoencoder class added. Runs simple cases. Need to expand to more general, complex cases.
</commit_message>
<xml_diff>
--- a/data/weather/standard_profiles/Standard Profiles.xlsx
+++ b/data/weather/standard_profiles/Standard Profiles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\GitHub\weather\data\weather\standard_profiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C233A0-E4A2-4A57-ACCD-EBC3BD5F41C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B0229F-7133-4D11-ACFE-ECB82CFA2988}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25598" windowHeight="11550" activeTab="2" xr2:uid="{E751E42B-8441-4F50-9123-C41EFFF043F1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="11550" activeTab="2" xr2:uid="{E751E42B-8441-4F50-9123-C41EFFF043F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Standard Temperature" sheetId="1" r:id="rId1"/>
@@ -513,12 +513,12 @@
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
@@ -530,7 +530,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="9">
         <v>-1000</v>
       </c>
@@ -542,7 +542,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="10">
         <v>0</v>
       </c>
@@ -554,7 +554,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
         <v>1000</v>
       </c>
@@ -566,7 +566,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="10">
         <v>2000</v>
       </c>
@@ -578,7 +578,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="10">
         <v>3000</v>
       </c>
@@ -590,7 +590,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="10">
         <v>4000</v>
       </c>
@@ -602,7 +602,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="10">
         <v>5000</v>
       </c>
@@ -614,7 +614,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="10">
         <v>6000</v>
       </c>
@@ -626,7 +626,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="10">
         <v>7000</v>
       </c>
@@ -638,7 +638,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
         <v>8000</v>
       </c>
@@ -650,7 +650,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
         <v>9000</v>
       </c>
@@ -662,7 +662,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="10">
         <v>10000</v>
       </c>
@@ -674,7 +674,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="10">
         <v>15000</v>
       </c>
@@ -686,7 +686,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="10">
         <v>20000</v>
       </c>
@@ -698,7 +698,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="10">
         <v>25000</v>
       </c>
@@ -710,7 +710,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="10">
         <v>30000</v>
       </c>
@@ -722,7 +722,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="10">
         <v>40000</v>
       </c>
@@ -734,7 +734,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="10">
         <v>50000</v>
       </c>
@@ -746,7 +746,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="10">
         <v>60000</v>
       </c>
@@ -758,7 +758,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="10">
         <v>70000</v>
       </c>
@@ -770,7 +770,7 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="10">
         <v>80000</v>
       </c>
@@ -782,7 +782,7 @@
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="7"/>
@@ -804,12 +804,12 @@
       <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.796875" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -817,7 +817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -825,7 +825,7 @@
         <v>59.62</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>304.8</v>
       </c>
@@ -833,7 +833,7 @@
         <v>60.48</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>609.6</v>
       </c>
@@ -841,7 +841,7 @@
         <v>62.03</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>914.4</v>
       </c>
@@ -849,7 +849,7 @@
         <v>63.83</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>1219.2</v>
       </c>
@@ -857,7 +857,7 @@
         <v>65.569999999999993</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>1524</v>
       </c>
@@ -865,7 +865,7 @@
         <v>67.06</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>1828.8</v>
       </c>
@@ -873,7 +873,7 @@
         <v>68.2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>2133.6</v>
       </c>
@@ -881,7 +881,7 @@
         <v>68.97</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>2438.4</v>
       </c>
@@ -889,7 +889,7 @@
         <v>69.41</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>2743.2</v>
       </c>
@@ -897,7 +897,7 @@
         <v>69.62</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>3048</v>
       </c>
@@ -905,7 +905,7 @@
         <v>69.72</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>3352.8</v>
       </c>
@@ -913,7 +913,7 @@
         <v>69.83</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>3657.6</v>
       </c>
@@ -921,7 +921,7 @@
         <v>70.05</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>3962.4</v>
       </c>
@@ -929,7 +929,7 @@
         <v>70.459999999999994</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>4267.2</v>
       </c>
@@ -937,7 +937,7 @@
         <v>71.12</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>4572</v>
       </c>
@@ -945,7 +945,7 @@
         <v>72.040000000000006</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>4876.8</v>
       </c>
@@ -953,7 +953,7 @@
         <v>73.19</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>5181.6000000000004</v>
       </c>
@@ -961,7 +961,7 @@
         <v>74.48</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>5486.4</v>
       </c>
@@ -969,7 +969,7 @@
         <v>75.77</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>5791.2</v>
       </c>
@@ -977,7 +977,7 @@
         <v>76.900000000000006</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>6096</v>
       </c>
@@ -985,7 +985,7 @@
         <v>77.61</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>6400.8</v>
       </c>
@@ -993,7 +993,7 @@
         <v>77.66</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>6705.6</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>76.77</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>7010.4</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>74.75</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>7315.2</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>71.47</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>7620</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>66.959999999999994</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>7924.8</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>61.38</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>8229.6</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>55.07</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>8534.4</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>48.44</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>8839.2000000000007</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>41.95</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>9144</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>36.01</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>9448.7999999999993</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>30.95</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>9753.6</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>27.01</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>10058.4</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>24.38</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>10363.200000000001</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>23.31</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>10668</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>24.29</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>10972.8</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>28.6</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>11277.6</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>25.61</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>11582.4</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>22.1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>11887.2</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>19.04</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>12192</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>16.420000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>12496.8</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>12801.6</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>12.34</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>13106.4</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>13411.2</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>9.5299999999999994</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>13716</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>8.49</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>14020.8</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>7.64</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>14325.6</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>6.95</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>14630.4</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>14935.2</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>5.97</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>15240</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>5.63</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>15544.8</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>5.38</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>16154.4</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>5.08</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>16459.2</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>5.0199999999999996</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>16764</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>5.01</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>17068.8</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>5.03</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>17373.599999999999</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>5.09</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>17678.400000000001</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>5.18</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>17983.2</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>5.28</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>18288</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>18592.8</v>
       </c>
@@ -1315,16 +1315,16 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.9296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="18">
         <v>-1000</v>
       </c>
@@ -1361,7 +1361,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="19">
         <v>0</v>
       </c>
@@ -1384,7 +1384,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="19">
         <v>1000</v>
       </c>
@@ -1407,7 +1407,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="19">
         <v>2000</v>
       </c>
@@ -1430,7 +1430,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="19">
         <v>3000</v>
       </c>
@@ -1453,7 +1453,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="19">
         <v>4000</v>
       </c>
@@ -1476,7 +1476,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="19">
         <v>5000</v>
       </c>
@@ -1499,7 +1499,7 @@
       <c r="K8" s="1"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="19">
         <v>6000</v>
       </c>
@@ -1522,7 +1522,7 @@
       <c r="K9" s="1"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="19">
         <v>7000</v>
       </c>
@@ -1545,7 +1545,7 @@
       <c r="K10" s="1"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="19">
         <v>8000</v>
       </c>
@@ -1568,7 +1568,7 @@
       <c r="K11" s="1"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="19">
         <v>9000</v>
       </c>
@@ -1591,7 +1591,7 @@
       <c r="K12" s="1"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="19">
         <v>10000</v>
       </c>
@@ -1614,7 +1614,7 @@
       <c r="K13" s="1"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="19">
         <v>15000</v>
       </c>
@@ -1637,7 +1637,7 @@
       <c r="K14" s="1"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="19">
         <v>20000</v>
       </c>
@@ -1660,7 +1660,7 @@
       <c r="K15" s="1"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="19">
         <v>25000</v>
       </c>
@@ -1683,7 +1683,7 @@
       <c r="K16" s="1"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="19">
         <v>30000</v>
       </c>
@@ -1706,7 +1706,7 @@
       <c r="K17" s="1"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="19">
         <v>40000</v>
       </c>
@@ -1729,7 +1729,7 @@
       <c r="K18" s="1"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="19">
         <v>50000</v>
       </c>
@@ -1752,7 +1752,7 @@
       <c r="K19" s="1"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="19">
         <v>60000</v>
       </c>
@@ -1775,7 +1775,7 @@
       <c r="K20" s="1"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="19">
         <v>70000</v>
       </c>
@@ -1798,7 +1798,7 @@
       <c r="K21" s="1"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="19">
         <v>80000</v>
       </c>
@@ -1821,7 +1821,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="14"/>
@@ -1840,7 +1840,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>

</xml_diff>